<commit_message>
Update flight types and Wizzair daily reports
</commit_message>
<xml_diff>
--- a/izvještaji/generated/BHDCA_January_2026.xlsx
+++ b/izvještaji/generated/BHDCA_January_2026.xlsx
@@ -3262,13 +3262,13 @@
       </c>
       <c r="E20" s="308" t="n"/>
       <c r="F20" s="65" t="n">
-        <v>206</v>
+        <v>164</v>
       </c>
       <c r="G20" s="65" t="n">
-        <v>100</v>
+        <v>55</v>
       </c>
       <c r="H20" s="65" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I20" s="65">
         <f>SUM(G20,H20)</f>
@@ -3346,13 +3346,13 @@
       </c>
       <c r="E22" s="308" t="n"/>
       <c r="F22" s="67" t="n">
-        <v>206</v>
+        <v>164</v>
       </c>
       <c r="G22" s="67" t="n">
-        <v>100</v>
+        <v>55</v>
       </c>
       <c r="H22" s="67" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I22" s="65">
         <f>SUM(G22,H22)</f>
@@ -3430,13 +3430,13 @@
       </c>
       <c r="E24" s="308" t="n"/>
       <c r="F24" s="67" t="n">
-        <v>206</v>
+        <v>164</v>
       </c>
       <c r="G24" s="67" t="n">
-        <v>100</v>
+        <v>55</v>
       </c>
       <c r="H24" s="67" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I24" s="65">
         <f>SUM(G24,H24)</f>

</xml_diff>